<commit_message>
created class for sidebar and sarch in loan entry and loan review.
</commit_message>
<xml_diff>
--- a/kcredit/src/test/resources/FlatfileAutomation.xlsx
+++ b/kcredit/src/test/resources/FlatfileAutomation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokulrajkaleidofin\JavaProjects\kcredit\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokulrajkaleidofin\git\KcreditTest\kcredit\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7AB4915-771E-49C9-8EEF-6875A8BB777A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28575452-3B56-48F3-91DA-BB0EFA1469C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{DBB5038C-763A-4255-9F82-1D3B033B2A2F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBB5038C-763A-4255-9F82-1D3B033B2A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="LOGINCREDS" sheetId="1" r:id="rId1"/>
@@ -36,30 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>username</t>
+    <t>mobilnumber</t>
   </si>
   <si>
-    <t>password</t>
+    <t>partnerloanid</t>
   </si>
   <si>
-    <t>Valid</t>
-  </si>
-  <si>
-    <t>gkcpl</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>gypl</t>
-  </si>
-  <si>
-    <t>Admin1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid </t>
+    <t>pasrtnercustomerid</t>
   </si>
 </sst>
 </file>
@@ -418,56 +403,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9978F5-649F-4E54-867E-3226C29018A0}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>88833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created method for partners dropdown in loanentry and loanreview screen
</commit_message>
<xml_diff>
--- a/kcredit/src/test/resources/FlatfileAutomation.xlsx
+++ b/kcredit/src/test/resources/FlatfileAutomation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokulrajkaleidofin\git\KcreditTest\kcredit\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28575452-3B56-48F3-91DA-BB0EFA1469C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D97B02C-1790-4D95-B2DC-66536322FE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBB5038C-763A-4255-9F82-1D3B033B2A2F}"/>
   </bookViews>
   <sheets>
-    <sheet name="LOGINCREDS" sheetId="1" r:id="rId1"/>
+    <sheet name="logincrds" sheetId="1" r:id="rId1"/>
+    <sheet name="partners" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>mobilnumber</t>
   </si>
@@ -45,13 +46,127 @@
   </si>
   <si>
     <t>pasrtnercustomerid</t>
+  </si>
+  <si>
+    <t>sonata</t>
+  </si>
+  <si>
+    <t>Samasta</t>
+  </si>
+  <si>
+    <t>Pahal</t>
+  </si>
+  <si>
+    <t>Cashpor</t>
+  </si>
+  <si>
+    <t>Magalir</t>
+  </si>
+  <si>
+    <t>loadtestingpartner11</t>
+  </si>
+  <si>
+    <t>loadtestingpartner12</t>
+  </si>
+  <si>
+    <t>loadtestingpartner13</t>
+  </si>
+  <si>
+    <t>loadtestingpartner14</t>
+  </si>
+  <si>
+    <t>loadtestingpartner15</t>
+  </si>
+  <si>
+    <t>Sugmya</t>
+  </si>
+  <si>
+    <t>1M2S3M</t>
+  </si>
+  <si>
+    <t>subhlakshmi</t>
+  </si>
+  <si>
+    <t>CTL</t>
+  </si>
+  <si>
+    <t>Samavesh PR</t>
+  </si>
+  <si>
+    <t>Svasti Microfinance</t>
+  </si>
+  <si>
+    <t>Mitrata</t>
+  </si>
+  <si>
+    <t>SWARA FINCARE LIMITED</t>
+  </si>
+  <si>
+    <t>Seeds Fincap</t>
+  </si>
+  <si>
+    <t>Subhlakshmi Finance Pvt Ltd</t>
+  </si>
+  <si>
+    <t>Maximal</t>
+  </si>
+  <si>
+    <t>Kiara</t>
+  </si>
+  <si>
+    <t>IREP</t>
+  </si>
+  <si>
+    <t>Midland_test</t>
+  </si>
+  <si>
+    <t>Sonata PR</t>
+  </si>
+  <si>
+    <t>Magalir PR</t>
+  </si>
+  <si>
+    <t>sona1ta1</t>
+  </si>
+  <si>
+    <t>Pahal PR</t>
+  </si>
+  <si>
+    <t>Sugmya PR</t>
+  </si>
+  <si>
+    <t>MSM</t>
+  </si>
+  <si>
+    <t>subhlakshmi PR</t>
+  </si>
+  <si>
+    <t>Capital Trust Limited PR</t>
+  </si>
+  <si>
+    <t>Svasti PR</t>
+  </si>
+  <si>
+    <t>samavesh</t>
+  </si>
+  <si>
+    <t>Mitrata PR</t>
+  </si>
+  <si>
+    <t>MIDLAND_MICROFIN_LIMITED</t>
+  </si>
+  <si>
+    <t>MAXIMAL-KISCORE</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,8 +174,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -70,6 +191,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -86,9 +213,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,18 +537,18 @@
   <dimension ref="B1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.26953125" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +559,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>88833</v>
       </c>
@@ -436,4 +567,213 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E86205-D948-4E0C-92BB-266EE8B35B0A}">
+  <dimension ref="A1:A38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" activeCellId="1" sqref="A1 C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created Approval MIS report functionality and loanEntry.missingfeields
</commit_message>
<xml_diff>
--- a/kcredit/src/test/resources/FlatfileAutomation.xlsx
+++ b/kcredit/src/test/resources/FlatfileAutomation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokulrajkaleidofin\git\KcreditTest\kcredit\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D97B02C-1790-4D95-B2DC-66536322FE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2D4B5E-1C55-45FE-8334-6FD953373BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBB5038C-763A-4255-9F82-1D3B033B2A2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{DBB5038C-763A-4255-9F82-1D3B033B2A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="logincrds" sheetId="1" r:id="rId1"/>
     <sheet name="partners" sheetId="2" r:id="rId2"/>
+    <sheet name="loandetails" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>mobilnumber</t>
   </si>
@@ -160,6 +161,21 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>mobilenumber</t>
+  </si>
+  <si>
+    <t>partnercustomerid</t>
+  </si>
+  <si>
+    <t>testAutomationg001</t>
+  </si>
+  <si>
+    <t>6000010000</t>
+  </si>
+  <si>
+    <t>groupid</t>
   </si>
 </sst>
 </file>
@@ -213,13 +229,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9978F5-649F-4E54-867E-3226C29018A0}">
   <dimension ref="B1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -573,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E86205-D948-4E0C-92BB-266EE8B35B0A}">
   <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" activeCellId="1" sqref="A1 C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -776,4 +793,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CF095D-5981-4E05-A0D3-2F011DEDD3A9}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="25.90625" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implimented clicktocategoriesMethod for 	Agentinfo 	Basic category info
</commit_message>
<xml_diff>
--- a/kcredit/src/test/resources/FlatfileAutomation.xlsx
+++ b/kcredit/src/test/resources/FlatfileAutomation.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokulrajkaleidofin\git\KcreditTest\kcredit\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF2D4B5E-1C55-45FE-8334-6FD953373BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D807A13-FF13-437C-BBD2-B5722B7D3AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{DBB5038C-763A-4255-9F82-1D3B033B2A2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{DBB5038C-763A-4255-9F82-1D3B033B2A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="logincrds" sheetId="1" r:id="rId1"/>
     <sheet name="partners" sheetId="2" r:id="rId2"/>
     <sheet name="loandetails" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>mobilnumber</t>
   </si>
@@ -176,6 +177,27 @@
   </si>
   <si>
     <t>groupid</t>
+  </si>
+  <si>
+    <t>testAutomationg002</t>
+  </si>
+  <si>
+    <t>testAutomationg003</t>
+  </si>
+  <si>
+    <t>6000010001</t>
+  </si>
+  <si>
+    <t>6000010002</t>
+  </si>
+  <si>
+    <t>sanjay</t>
+  </si>
+  <si>
+    <t>gokul</t>
+  </si>
+  <si>
+    <t>mobile</t>
   </si>
 </sst>
 </file>
@@ -229,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -237,6 +259,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E86205-D948-4E0C-92BB-266EE8B35B0A}">
   <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -797,11 +820,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CF095D-5981-4E05-A0D3-2F011DEDD3A9}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -839,7 +860,96 @@
         <v>43</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9B0CF1-8B7E-4286-BA2D-7FDE1EAD53EE}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="45.453125" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
developed end to end method
</commit_message>
<xml_diff>
--- a/kcredit/src/test/resources/FlatfileAutomation.xlsx
+++ b/kcredit/src/test/resources/FlatfileAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokulrajkaleidofin\git\KcreditTest\kcredit\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D807A13-FF13-437C-BBD2-B5722B7D3AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C4E366-3973-4C7B-B720-1C4908EE45B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{DBB5038C-763A-4255-9F82-1D3B033B2A2F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{DBB5038C-763A-4255-9F82-1D3B033B2A2F}"/>
   </bookViews>
   <sheets>
     <sheet name="logincrds" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
   <si>
     <t>mobilnumber</t>
   </si>
@@ -170,34 +170,46 @@
     <t>partnercustomerid</t>
   </si>
   <si>
+    <t>groupid</t>
+  </si>
+  <si>
+    <t>testAutomationg003</t>
+  </si>
+  <si>
+    <t>6000010002</t>
+  </si>
+  <si>
+    <t>sanjay</t>
+  </si>
+  <si>
+    <t>gokul</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>6000010005</t>
+  </si>
+  <si>
+    <t>testAutomationg005</t>
+  </si>
+  <si>
     <t>testAutomationg001</t>
   </si>
   <si>
     <t>6000010000</t>
   </si>
   <si>
-    <t>groupid</t>
-  </si>
-  <si>
     <t>testAutomationg002</t>
   </si>
   <si>
-    <t>testAutomationg003</t>
-  </si>
-  <si>
     <t>6000010001</t>
   </si>
   <si>
-    <t>6000010002</t>
-  </si>
-  <si>
-    <t>sanjay</t>
-  </si>
-  <si>
-    <t>gokul</t>
-  </si>
-  <si>
-    <t>mobile</t>
+    <t>testAutomationg006</t>
+  </si>
+  <si>
+    <t>6000010006</t>
   </si>
 </sst>
 </file>
@@ -822,7 +834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1CF095D-5981-4E05-A0D3-2F011DEDD3A9}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -843,71 +857,77 @@
         <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -919,8 +939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9B0CF1-8B7E-4286-BA2D-7FDE1EAD53EE}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -931,18 +951,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>888</v>

</xml_diff>